<commit_message>
Update 0. CTRL-E Autofill Example.xlsx
</commit_message>
<xml_diff>
--- a/0. CTRL-E Autofill Example.xlsx
+++ b/0. CTRL-E Autofill Example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alphad-my.sharepoint.com/personal/alexwirtz_alphadevelopment_com/Documents/Desktop/bofaoffcycleinterns/Delegate Exercises/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GeorgeMount\Documents\GitHub\hsbc-enhancing-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{52988E0A-8014-43E0-BF22-52E1CE7D96EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82B05EBD-8900-4C75-A852-7515C712F2EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8291DE-A99E-48F2-BCCB-96CD7859D436}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25728" yWindow="2688" windowWidth="19092" windowHeight="12492" xr2:uid="{166EB4FE-D252-4148-AB66-032525DDAAA0}"/>
+    <workbookView xWindow="2843" yWindow="518" windowWidth="21622" windowHeight="11205" xr2:uid="{166EB4FE-D252-4148-AB66-032525DDAAA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Given Name</t>
   </si>
@@ -74,7 +74,16 @@
     <t>abel.baker@xyz.com</t>
   </si>
   <si>
-    <t>The CTRL-E Autofill Hack</t>
+    <t>1. Use flash fill to complete these emails @xyz.com</t>
+  </si>
+  <si>
+    <t>2. Create a new custom list for the fill handle:</t>
+  </si>
+  <si>
+    <t>Instructions are at https://support.microsoft.com/en-us/office/create-or-delete-a-custom-list-for-sorting-and-filling-data-d1cf624f-2d2b-44fa-814b-ba213ec2fd61</t>
+  </si>
+  <si>
+    <t>Examples: Small/Medium/Large, North/East/South/West, etc.</t>
   </si>
 </sst>
 </file>
@@ -140,10 +149,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -455,25 +460,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8F6AEE0-CE66-4324-8B20-947748ED0FBC}">
-  <dimension ref="B2:D8"/>
+  <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="146" zoomScaleNormal="146" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.90625" customWidth="1"/>
-    <col min="3" max="3" width="13.26953125" customWidth="1"/>
-    <col min="4" max="4" width="20.26953125" customWidth="1"/>
+    <col min="2" max="2" width="12.9296875" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" customWidth="1"/>
+    <col min="4" max="4" width="20.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -484,7 +487,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -495,7 +498,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -504,7 +507,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -513,7 +516,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>9</v>
       </c>
@@ -521,6 +524,21 @@
         <v>10</v>
       </c>
       <c r="D8" s="1"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -534,28 +552,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="059fecdb-ee26-4135-81c8-712a955c51df" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="26d2fa48-a9bb-4686-8122-5406e5c0c038">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100265553BD9181624686A68F63ABB446DF" ma:contentTypeVersion="21" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ee33f439afe5f713e430bc419b9183ba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="26d2fa48-a9bb-4686-8122-5406e5c0c038" xmlns:ns3="059fecdb-ee26-4135-81c8-712a955c51df" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8a55f4bd9fbe5a9e1352735377af3810" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -821,10 +817,44 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="059fecdb-ee26-4135-81c8-712a955c51df" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="26d2fa48-a9bb-4686-8122-5406e5c0c038">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA72A566-AE98-4B1A-877C-A23B36A21408}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E560EAAF-0EC4-494B-ACEA-355A04770B03}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="26d2fa48-a9bb-4686-8122-5406e5c0c038"/>
+    <ds:schemaRef ds:uri="059fecdb-ee26-4135-81c8-712a955c51df"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -842,5 +872,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E560EAAF-0EC4-494B-ACEA-355A04770B03}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DA72A566-AE98-4B1A-877C-A23B36A21408}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>